<commit_message>
Ajout histogramme pour loi normale
</commit_message>
<xml_diff>
--- a/rapportExcel.xlsx
+++ b/rapportExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanl\OneDrive\Bureau\IFT-3913_qualité\tp\tp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD69DE06-DAB5-411E-B8DF-C1944F7034B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49803C23-206A-44A0-82F0-58DFF62D7451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{82D28E78-B979-4489-BC9F-74488EDAABCA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="861" activeTab="8" xr2:uid="{82D28E78-B979-4489-BC9F-74488EDAABCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,37 @@
     <sheet name="Graphique3" sheetId="4" r:id="rId4"/>
     <sheet name="Graphique4" sheetId="5" r:id="rId5"/>
     <sheet name="Graphique5" sheetId="6" r:id="rId6"/>
+    <sheet name="Graphique6" sheetId="7" r:id="rId7"/>
+    <sheet name="Graphique7" sheetId="8" r:id="rId8"/>
+    <sheet name="histogramme_DCP" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$B$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$B$2:$B$633</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Feuil1!$B$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Feuil1!$B$2:$B$633</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Feuil1!$B$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Feuil1!$B$2:$B$633</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Feuil1!$B$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Feuil1!$B$2:$B$633</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Feuil1!$B$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Feuil1!$B$2:$B$633</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Feuil1!$B$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Feuil1!$B$2:$B$633</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$C$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Feuil1!$C$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Feuil1!$C$2:$C$633</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Feuil1!$D$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Feuil1!$D$2:$D$633</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Feuil1!$D$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Feuil1!$D$2:$D$633</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Feuil1!$C$2:$C$633</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Feuil1!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Feuil1!$C$2:$C$633</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Feuil1!$D$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Feuil1!$D$2:$D$633</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Feuil1!$D$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Feuil1!$D$2:$D$633</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Feuil1!$B$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Feuil1!$B$2:$B$633</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Feuil1!$B$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Feuil1!$B$2:$B$633</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -10909,6 +10930,234 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
@@ -11132,7 +11381,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -11170,7 +11419,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{749993DD-B70D-4A8B-92C0-8FBCFCE4F36D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v> DCP</cx:v>
             </cx:txData>
           </cx:tx>
@@ -11204,6 +11453,207 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="1.10000002"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>NOCom</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>NOCom</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{C9833529-1CC5-4B92-BB45-6E400E06EBA6}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:v> NOCom</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.21</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>NCLOC</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>NCLOC</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{2A18BCDF-6DB0-445F-BD86-DCD3AD92E4F0}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:v> NCLOC</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.25</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>DCP</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>DCP</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{C839821A-0FA5-452B-8058-8AA2D286182B}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.24</cx:f>
+              <cx:v> DCP</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
@@ -11377,6 +11827,126 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -13962,6 +14532,1659 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="369">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" cap="none" spc="20"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="369">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" cap="none" spc="20"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="369">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" cap="none" spc="20"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{75F4CD8F-09CB-4947-8F9A-ED49A4614BE0}">
   <sheetPr/>
@@ -14011,6 +16234,39 @@
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="80" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{56957406-2CB8-41B9-911F-B9BFDD9B4DD7}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="80" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{9AF7533A-6D5D-4556-BAA8-8A393C07F128}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="80" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{4D5326C2-DB5A-4680-B011-1639D40C80E5}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14071,6 +16327,285 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D40BFED-9C3E-C691-0DF7-07091A09F404}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr>
+          <a:spLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noTextEdit="1"/>
+        </cdr:cNvSpPr>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="8657422" cy="6279614"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstClr val="white"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="1">
+          <a:solidFill>
+            <a:prstClr val="green"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" horzOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="fr-CA" sz="1100"/>
+            <a:t>Ce graphique n’est pas disponible dans votre version d’Excel.
+La modification de cette forme ou l’enregistrement de ce classeur dans un autre format de fichier endommagera le graphique de façon irréparable.</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8657422" cy="6279614"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Graphique 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DCAADB6-A95A-4740-85ED-87937F2E8DA0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks/>
+            </xdr:cNvGraphicFramePr>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+              <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB75A3FF-D094-4E22-A12A-5CFC2B5EB7AC}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr>
+          <a:spLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noTextEdit="1"/>
+        </cdr:cNvSpPr>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="8657422" cy="6279614"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstClr val="white"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="1">
+          <a:solidFill>
+            <a:prstClr val="green"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" horzOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="fr-CA" sz="1100"/>
+            <a:t>Ce graphique n’est pas disponible dans votre version d’Excel.
+La modification de cette forme ou l’enregistrement de ce classeur dans un autre format de fichier endommagera le graphique de façon irréparable.</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8657422" cy="6279614"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Graphique 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC8D1947-35F3-356B-8975-1F8B98A52909}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks/>
+            </xdr:cNvGraphicFramePr>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+              <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86DB32C4-3B98-ABCF-27BF-8338E6E8CB3E}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr>
+          <a:spLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noTextEdit="1"/>
+        </cdr:cNvSpPr>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="8657422" cy="6279614"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstClr val="white"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="1">
+          <a:solidFill>
+            <a:prstClr val="green"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" horzOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="fr-CA" sz="1100"/>
+            <a:t>Ce graphique n’est pas disponible dans votre version d’Excel.
+La modification de cette forme ou l’enregistrement de ce classeur dans un autre format de fichier endommagera le graphique de façon irréparable.</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
@@ -14087,7 +16622,7 @@
         <cdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7946766-EBFD-2FC5-C1FB-DA57D4F941F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99FB964A-A58B-8C7A-851D-B701A0D88DE4}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -14198,7 +16733,7 @@
         <cdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67673CAA-BA91-E501-8A6A-E217CAAD4249}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9D860B3-DA9A-6C21-C03E-99903B1BFF54}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -14309,7 +16844,7 @@
         <cdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55F1C89E-ADC2-1EAD-7843-1FD95B0A753A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A99ADACB-C30E-462F-B162-77839E904B82}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -14411,6 +16946,60 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8657422" cy="6279614"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Graphique 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{552CCA7D-DC76-9487-38AF-10646D143EE5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks/>
+            </xdr:cNvGraphicFramePr>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+              <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
@@ -14715,8 +17304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C9F10E-7996-4A16-ABA1-95A07A8A4C34}">
   <dimension ref="A1:H633"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>